<commit_message>
Ajuste al modelo - medidores y polizas many to one
</commit_message>
<xml_diff>
--- a/hidromed/static/archivos/Usuarios.xlsx
+++ b/hidromed/static/archivos/Usuarios.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
-  <si>
-    <t xml:space="preserve">ID NIT Empresa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empresa</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+  <si>
+    <t xml:space="preserve">ID NIT Acueducto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acueducto</t>
   </si>
   <si>
     <t xml:space="preserve">Póliza</t>
@@ -34,7 +34,16 @@
     <t xml:space="preserve">Serial Medidor</t>
   </si>
   <si>
-    <t xml:space="preserve">Nombre Usuario</t>
+    <t xml:space="preserve">Cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nit/CC Cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dirección Cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuario Acceso</t>
   </si>
   <si>
     <t xml:space="preserve">Imaginamos</t>
@@ -46,6 +55,12 @@
     <t xml:space="preserve">C11LA004183</t>
   </si>
   <si>
+    <t xml:space="preserve">Supermercado 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calle 3 3 – 56</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fernando Perez</t>
   </si>
   <si>
@@ -55,6 +70,9 @@
     <t xml:space="preserve">C15LA345678</t>
   </si>
   <si>
+    <t xml:space="preserve">Manuel Espinoza</t>
+  </si>
+  <si>
     <t xml:space="preserve">Globan</t>
   </si>
   <si>
@@ -62,6 +80,12 @@
   </si>
   <si>
     <t xml:space="preserve">00014337</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industria 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calle 30 # 21 26</t>
   </si>
   <si>
     <t xml:space="preserve">Dario Guerrero</t>
@@ -270,23 +294,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4534412955466"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.497975708502"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.17004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6963562753036"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="16.2388663967611"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -301,6 +325,15 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -308,16 +341,25 @@
         <v>830300412</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>800123222</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -325,33 +367,51 @@
         <v>830300412</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>800123222</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>900890789</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>900123123</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -359,16 +419,25 @@
         <v>900890789</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>900123123</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificación archivo de usuarios gráfico template
</commit_message>
<xml_diff>
--- a/hidromed/static/archivos/Usuarios.xlsx
+++ b/hidromed/static/archivos/Usuarios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">ID NIT Acueducto</t>
   </si>
@@ -44,60 +44,6 @@
   </si>
   <si>
     <t xml:space="preserve">Usuario Acceso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imaginamos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00889933</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C11LA004183</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supermercado 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calle 3 3 – 56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fernando Perez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00897899</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C15LA345678</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manuel Espinoza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Globan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">234122344</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00014337</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Industria 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calle 30 # 21 26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dario Guerrero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">111122335</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00014338</t>
-  </si>
-  <si>
-    <t xml:space="preserve">francisco.morales</t>
   </si>
 </sst>
 </file>
@@ -294,20 +240,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4534412955466"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.17004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6963562753036"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="16.2388663967611"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4615384615385"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.246963562753"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -337,108 +283,14 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
-        <v>830300412</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>800123222</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
-        <v>830300412</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>800123222</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
-        <v>900890789</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>900123123</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
-        <v>900890789</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>900123123</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>